<commit_message>
- Dev mode now mutes all sounds after escape is pressed once to exit a map - Update bugs and requests
</commit_message>
<xml_diff>
--- a/latestBuild/EngineBugAndRequest.xlsx
+++ b/latestBuild/EngineBugAndRequest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">ISSUE</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">STATUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need to make music mute-able</t>
   </si>
   <si>
     <t xml:space="preserve">Tile vs absolute offset for movement</t>
@@ -149,7 +146,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -174,19 +171,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Adds support for party management and export in town
- Fix bug where planner explodes when a save is attempted on a resource
that has never been accessed in the UI
- DevParams are now in XML formatted and must be generated by the engine
(see above)
- Trigger file should no longer be clobbered if an error occurs during
saving
- Fix bug where heroes menu does not scroll correctly when you have a
large party
- Fix bug where priest displays "no promotion" text after a promotion
- DevParams are now ONLY loaded for battles
- Bump Engine Version
</commit_message>
<xml_diff>
--- a/latestBuild/EngineBugAndRequest.xlsx
+++ b/latestBuild/EngineBugAndRequest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">ISSUE</t>
   </si>
@@ -38,6 +38,27 @@
   </si>
   <si>
     <t xml:space="preserve">Check move immediately</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Separate Weapon Animation from Hero Animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discrete animation for heroes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Animator portraits are still needed, but should be their own output so that each import doesn’t require re-sizing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decide if spells should be split out in the animations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level up/level down/reset sprite items or menu debug menu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select battle text file in development mode</t>
   </si>
 </sst>
 </file>
@@ -52,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -73,6 +95,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,15 +166,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="99.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="99.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
@@ -179,6 +202,39 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Adds enemy vision and triggers to change it - Add wander AI approach - Add AI Jank (10%) - Casters only have magic shields if they use or can use staffs or wands - AI debug now shows above foreground - AI debug now shows vision
</commit_message>
<xml_diff>
--- a/latestBuild/EngineBugAndRequest.xlsx
+++ b/latestBuild/EngineBugAndRequest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t xml:space="preserve">ISSUE</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Separate Weapon Animation from Hero Animation</t>
   </si>
   <si>
+    <t xml:space="preserve">DONE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Discrete animation for heroes</t>
   </si>
   <si>
@@ -55,10 +58,22 @@
     <t xml:space="preserve">Level up/level down/reset sprite items or menu debug menu. </t>
   </si>
   <si>
-    <t xml:space="preserve">DONE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Select battle text file in development mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts for items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find better way to show shield in DodgeCombatAnimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add jank AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add wander approach type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add AI vision</t>
   </si>
 </sst>
 </file>
@@ -68,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -93,6 +108,20 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1B75BC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0066B3"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -140,12 +169,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -158,6 +195,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF1B75BC"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066B3"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -166,10 +263,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -205,36 +302,73 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="A9" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>